<commit_message>
TMB with full RE
</commit_message>
<xml_diff>
--- a/code/samples_summary_inference.xlsx
+++ b/code/samples_summary_inference.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morril01/Documents/PhD/GlobalDA/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF908A7F-9B59-864E-9BC1-B89950A30F08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9755E445-4CA6-E140-8DA0-6936092DA277}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="21460" windowWidth="27640" windowHeight="17540" xr2:uid="{5DBFF44D-DF5C-A046-9A50-B35ED57F5618}"/>
+    <workbookView xWindow="1760" yWindow="2280" windowWidth="27640" windowHeight="16720" xr2:uid="{5DBFF44D-DF5C-A046-9A50-B35ED57F5618}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Full intercept" sheetId="4" r:id="rId1"/>
+    <sheet name="Single intercept" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="69">
   <si>
     <t>nuc1 TMB</t>
   </si>
@@ -199,13 +200,46 @@
   </si>
   <si>
     <t>if using intercept, I have had many Non-PD in DM!</t>
+  </si>
+  <si>
+    <t>Number of samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Error in nrow(i@count_matrices_all[[1]]) :    trying to get slot "count_matrices_all" from an object of a basic class ("logical") with no slots</t>
+  </si>
+  <si>
+    <t>With intercept: with intercept for beta</t>
+  </si>
+  <si>
+    <t>Without intercept: no intercept for beta</t>
+  </si>
+  <si>
+    <t>TMB</t>
+  </si>
+  <si>
+    <t>Stan only have one random effect</t>
+  </si>
+  <si>
+    <t>In either case, there is just one random effect (i.e. only last log-ratio changes with this intercept)</t>
+  </si>
+  <si>
+    <t>Number of params to infer M</t>
+  </si>
+  <si>
+    <t>Number of params to infer LNM</t>
+  </si>
+  <si>
+    <t>Number of params to infer DM</t>
+  </si>
+  <si>
+    <t>Number of signatures</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -225,6 +259,20 @@
       <sz val="120"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="30"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -357,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -399,6 +447,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,11 +776,1652 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CB1F27-3E1D-1D4A-838D-AA35D1F874EF}">
-  <dimension ref="A1:AC45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666FFE8A-0FBA-F94E-BAA2-6A7396674433}">
+  <dimension ref="A1:AA57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+      <selection activeCell="W35" sqref="W35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="17" thickBot="1">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" t="s">
+        <v>58</v>
+      </c>
+      <c r="T2" t="s">
+        <v>68</v>
+      </c>
+      <c r="U2" t="s">
+        <v>65</v>
+      </c>
+      <c r="V2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W2" t="s">
+        <v>67</v>
+      </c>
+      <c r="X2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="I3" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="43"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="43"/>
+      <c r="S3">
+        <v>15</v>
+      </c>
+      <c r="U3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="42"/>
+      <c r="G4" s="43"/>
+      <c r="I4" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="43"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="43"/>
+      <c r="S4">
+        <v>9</v>
+      </c>
+      <c r="U4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
+      <c r="I5" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="43"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="43"/>
+      <c r="S5">
+        <v>5</v>
+      </c>
+      <c r="U5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
+      <c r="I6" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="43"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="43"/>
+      <c r="S6">
+        <v>6</v>
+      </c>
+      <c r="U6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
+      <c r="I7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="43"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="43"/>
+      <c r="S7">
+        <v>27</v>
+      </c>
+      <c r="U7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
+      <c r="I8" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="43"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="43"/>
+      <c r="S8">
+        <v>136</v>
+      </c>
+      <c r="U8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
+      <c r="I9" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="43"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="43"/>
+      <c r="S9">
+        <v>2</v>
+      </c>
+      <c r="U9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
+      <c r="I10" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="43"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="43"/>
+      <c r="S10">
+        <v>8</v>
+      </c>
+      <c r="U10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="42"/>
+      <c r="G11" s="43"/>
+      <c r="I11" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="43"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="43"/>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="U11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="42"/>
+      <c r="G12" s="43"/>
+      <c r="I12" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="43"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="43"/>
+      <c r="S12">
+        <v>16</v>
+      </c>
+      <c r="U12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="42"/>
+      <c r="G13" s="43"/>
+      <c r="I13" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="43"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="43"/>
+      <c r="S13">
+        <v>34</v>
+      </c>
+      <c r="U13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="42"/>
+      <c r="G14" s="43"/>
+      <c r="I14" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="43"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="43"/>
+      <c r="S14">
+        <v>106</v>
+      </c>
+      <c r="U14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="42"/>
+      <c r="G15" s="43"/>
+      <c r="I15" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="43"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="43"/>
+      <c r="S15">
+        <v>15</v>
+      </c>
+      <c r="U15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="42"/>
+      <c r="G16" s="43"/>
+      <c r="I16" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="43"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="43"/>
+      <c r="S16">
+        <v>42</v>
+      </c>
+      <c r="U16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="42"/>
+      <c r="G17" s="43"/>
+      <c r="I17" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="43"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="43"/>
+      <c r="S17">
+        <v>37</v>
+      </c>
+      <c r="U17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="44" customHeight="1">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="42"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="5"/>
+      <c r="L18" s="43"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="43"/>
+      <c r="S18">
+        <v>65</v>
+      </c>
+      <c r="U18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="42"/>
+      <c r="G19" s="43"/>
+      <c r="I19" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="43"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="43"/>
+      <c r="S19">
+        <v>32</v>
+      </c>
+      <c r="U19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="42"/>
+      <c r="G20" s="43"/>
+      <c r="I20" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="43"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="43"/>
+      <c r="S20">
+        <v>38</v>
+      </c>
+      <c r="U20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="42"/>
+      <c r="G21" s="43"/>
+      <c r="I21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="43"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="43"/>
+      <c r="S21">
+        <v>86</v>
+      </c>
+      <c r="U21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="42"/>
+      <c r="G22" s="43"/>
+      <c r="I22" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="43"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="43"/>
+      <c r="S22">
+        <v>30</v>
+      </c>
+      <c r="U22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="42"/>
+      <c r="G23" s="43"/>
+      <c r="I23" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="43"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="43"/>
+      <c r="S23">
+        <v>207</v>
+      </c>
+      <c r="U23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="42"/>
+      <c r="G24" s="43"/>
+      <c r="I24" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="43"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="43"/>
+      <c r="S24">
+        <v>17</v>
+      </c>
+      <c r="U24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="42"/>
+      <c r="G25" s="43"/>
+      <c r="I25" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="5"/>
+      <c r="L25" s="43"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="43"/>
+      <c r="S25">
+        <v>34</v>
+      </c>
+      <c r="U25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="42"/>
+      <c r="G26" s="43"/>
+      <c r="I26" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" s="5"/>
+      <c r="L26" s="43"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="43"/>
+      <c r="S26">
+        <v>51</v>
+      </c>
+      <c r="U26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="42"/>
+      <c r="G27" s="43"/>
+      <c r="I27" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" s="5"/>
+      <c r="L27" s="43"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="43"/>
+      <c r="S27">
+        <v>53</v>
+      </c>
+      <c r="U27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="42"/>
+      <c r="G28" s="43"/>
+      <c r="I28" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K28" s="5"/>
+      <c r="L28" s="43"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="43"/>
+      <c r="S28">
+        <v>8</v>
+      </c>
+      <c r="U28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="42"/>
+      <c r="G29" s="43"/>
+      <c r="I29" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="5"/>
+      <c r="L29" s="43"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="43"/>
+      <c r="S29">
+        <v>19</v>
+      </c>
+      <c r="U29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="I30" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" s="5"/>
+      <c r="L30" s="43"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="43"/>
+      <c r="S30">
+        <v>97</v>
+      </c>
+      <c r="U30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="42"/>
+      <c r="G31" s="43"/>
+      <c r="I31" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" s="5"/>
+      <c r="L31" s="43"/>
+      <c r="N31" s="47"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="43"/>
+      <c r="S31">
+        <v>193</v>
+      </c>
+      <c r="U31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="42"/>
+      <c r="G32" s="43"/>
+      <c r="I32" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K32" s="5"/>
+      <c r="L32" s="43"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="43"/>
+      <c r="S32">
+        <v>70</v>
+      </c>
+      <c r="U32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="42"/>
+      <c r="G33" s="43"/>
+      <c r="I33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="5"/>
+      <c r="L33" s="43"/>
+      <c r="N33" s="47"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="43"/>
+      <c r="S33">
+        <v>208</v>
+      </c>
+      <c r="U33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="42"/>
+      <c r="G34" s="43"/>
+      <c r="I34" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J34" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K34" s="5"/>
+      <c r="L34" s="43"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="43"/>
+      <c r="S34">
+        <v>15</v>
+      </c>
+      <c r="U34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="42"/>
+      <c r="G35" s="43"/>
+      <c r="I35" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J35" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K35" s="5"/>
+      <c r="L35" s="43"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="43"/>
+      <c r="S35">
+        <v>30</v>
+      </c>
+      <c r="U35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="N36" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="O36" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="P36" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q36" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="S36" t="s">
+        <v>59</v>
+      </c>
+      <c r="U36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="42"/>
+      <c r="G37" s="43"/>
+      <c r="I37" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K37" s="5"/>
+      <c r="L37" s="43"/>
+      <c r="N37" s="47"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="43"/>
+      <c r="S37">
+        <v>15</v>
+      </c>
+      <c r="U37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="42"/>
+      <c r="G38" s="43"/>
+      <c r="I38" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J38" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K38" s="5"/>
+      <c r="L38" s="43"/>
+      <c r="N38" s="47"/>
+      <c r="O38" s="42"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="43"/>
+      <c r="S38">
+        <v>15</v>
+      </c>
+      <c r="U38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="42"/>
+      <c r="G39" s="43"/>
+      <c r="I39" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J39" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K39" s="5"/>
+      <c r="L39" s="43"/>
+      <c r="N39" s="47"/>
+      <c r="O39" s="42"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="43"/>
+      <c r="S39">
+        <v>30</v>
+      </c>
+      <c r="U39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="42"/>
+      <c r="G40" s="43"/>
+      <c r="I40" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J40" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K40" s="5"/>
+      <c r="L40" s="43"/>
+      <c r="N40" s="47"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="16"/>
+      <c r="Q40" s="43"/>
+      <c r="S40">
+        <v>41</v>
+      </c>
+      <c r="U40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="17" thickBot="1">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="45"/>
+      <c r="G41" s="46"/>
+      <c r="I41" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="J41" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="K41" s="12"/>
+      <c r="L41" s="46"/>
+      <c r="N41" s="48"/>
+      <c r="O41" s="45"/>
+      <c r="P41" s="44"/>
+      <c r="Q41" s="46"/>
+      <c r="S41">
+        <v>40</v>
+      </c>
+      <c r="U41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="26">
+      <c r="A44" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+    </row>
+    <row r="45" spans="1:21" ht="26">
+      <c r="A45" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="49"/>
+    </row>
+    <row r="46" spans="1:21" ht="26">
+      <c r="A46" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="49"/>
+    </row>
+    <row r="47" spans="1:21" ht="26">
+      <c r="A47" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="49"/>
+    </row>
+    <row r="48" spans="1:21" ht="26">
+      <c r="A48" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="49"/>
+      <c r="I48" s="49"/>
+    </row>
+    <row r="49" spans="1:27">
+      <c r="A49" s="50"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="50"/>
+      <c r="K49" s="50"/>
+      <c r="L49" s="50"/>
+      <c r="M49" s="50"/>
+      <c r="N49" s="50"/>
+      <c r="O49" s="50"/>
+      <c r="P49" s="50"/>
+      <c r="Q49" s="50"/>
+      <c r="R49" s="50"/>
+      <c r="S49" s="50"/>
+      <c r="T49" s="50"/>
+      <c r="U49" s="50"/>
+      <c r="V49" s="50"/>
+      <c r="W49" s="50"/>
+      <c r="X49" s="50"/>
+      <c r="Y49" s="50"/>
+      <c r="Z49" s="50"/>
+      <c r="AA49" s="50"/>
+    </row>
+    <row r="50" spans="1:27">
+      <c r="A50" s="50"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="50"/>
+      <c r="J50" s="50"/>
+      <c r="K50" s="50"/>
+      <c r="L50" s="50"/>
+      <c r="M50" s="50"/>
+      <c r="N50" s="50"/>
+      <c r="O50" s="50"/>
+      <c r="P50" s="50"/>
+      <c r="Q50" s="50"/>
+      <c r="R50" s="50"/>
+      <c r="S50" s="50"/>
+      <c r="T50" s="50"/>
+      <c r="U50" s="50"/>
+      <c r="V50" s="50"/>
+      <c r="W50" s="50"/>
+      <c r="X50" s="50"/>
+      <c r="Y50" s="50"/>
+      <c r="Z50" s="50"/>
+      <c r="AA50" s="50"/>
+    </row>
+    <row r="51" spans="1:27">
+      <c r="A51" s="50"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="50"/>
+      <c r="M51" s="50"/>
+      <c r="N51" s="50"/>
+      <c r="O51" s="50"/>
+      <c r="P51" s="50"/>
+      <c r="Q51" s="50"/>
+      <c r="R51" s="50"/>
+      <c r="S51" s="50"/>
+      <c r="T51" s="50"/>
+      <c r="U51" s="50"/>
+      <c r="V51" s="50"/>
+      <c r="W51" s="50"/>
+      <c r="X51" s="50"/>
+      <c r="Y51" s="50"/>
+      <c r="Z51" s="50"/>
+      <c r="AA51" s="50"/>
+    </row>
+    <row r="52" spans="1:27">
+      <c r="A52" s="50"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="50"/>
+      <c r="I52" s="50"/>
+      <c r="J52" s="50"/>
+      <c r="K52" s="50"/>
+      <c r="L52" s="50"/>
+      <c r="M52" s="50"/>
+      <c r="N52" s="50"/>
+      <c r="O52" s="50"/>
+      <c r="P52" s="50"/>
+      <c r="Q52" s="50"/>
+      <c r="R52" s="50"/>
+      <c r="S52" s="50"/>
+      <c r="T52" s="50"/>
+      <c r="U52" s="50"/>
+      <c r="V52" s="50"/>
+      <c r="W52" s="50"/>
+      <c r="X52" s="50"/>
+      <c r="Y52" s="50"/>
+      <c r="Z52" s="50"/>
+      <c r="AA52" s="50"/>
+    </row>
+    <row r="53" spans="1:27">
+      <c r="A53" s="50"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="50"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="50"/>
+      <c r="J53" s="50"/>
+      <c r="K53" s="50"/>
+      <c r="L53" s="50"/>
+      <c r="M53" s="50"/>
+      <c r="N53" s="50"/>
+      <c r="O53" s="50"/>
+      <c r="P53" s="50"/>
+      <c r="Q53" s="50"/>
+      <c r="R53" s="50"/>
+      <c r="S53" s="50"/>
+      <c r="T53" s="50"/>
+      <c r="U53" s="50"/>
+      <c r="V53" s="50"/>
+      <c r="W53" s="50"/>
+      <c r="X53" s="50"/>
+      <c r="Y53" s="50"/>
+      <c r="Z53" s="50"/>
+      <c r="AA53" s="50"/>
+    </row>
+    <row r="54" spans="1:27">
+      <c r="A54" s="50"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="50"/>
+      <c r="H54" s="50"/>
+      <c r="I54" s="50"/>
+      <c r="J54" s="50"/>
+      <c r="K54" s="50"/>
+      <c r="L54" s="50"/>
+      <c r="M54" s="50"/>
+      <c r="N54" s="50"/>
+      <c r="O54" s="50"/>
+      <c r="P54" s="50"/>
+      <c r="Q54" s="50"/>
+      <c r="R54" s="50"/>
+      <c r="S54" s="50"/>
+      <c r="T54" s="50"/>
+      <c r="U54" s="50"/>
+      <c r="V54" s="50"/>
+      <c r="W54" s="50"/>
+      <c r="X54" s="50"/>
+      <c r="Y54" s="50"/>
+      <c r="Z54" s="50"/>
+      <c r="AA54" s="50"/>
+    </row>
+    <row r="55" spans="1:27">
+      <c r="A55" s="50"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="50"/>
+      <c r="H55" s="50"/>
+      <c r="I55" s="50"/>
+      <c r="J55" s="50"/>
+      <c r="K55" s="50"/>
+      <c r="L55" s="50"/>
+      <c r="M55" s="50"/>
+      <c r="N55" s="50"/>
+      <c r="O55" s="50"/>
+      <c r="P55" s="50"/>
+      <c r="Q55" s="50"/>
+      <c r="R55" s="50"/>
+      <c r="S55" s="50"/>
+      <c r="T55" s="50"/>
+      <c r="U55" s="50"/>
+      <c r="V55" s="50"/>
+      <c r="W55" s="50"/>
+      <c r="X55" s="50"/>
+      <c r="Y55" s="50"/>
+      <c r="Z55" s="50"/>
+      <c r="AA55" s="50"/>
+    </row>
+    <row r="56" spans="1:27">
+      <c r="A56" s="50"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="50"/>
+      <c r="H56" s="50"/>
+      <c r="I56" s="50"/>
+      <c r="J56" s="50"/>
+      <c r="K56" s="50"/>
+      <c r="L56" s="50"/>
+      <c r="M56" s="50"/>
+      <c r="N56" s="50"/>
+      <c r="O56" s="50"/>
+      <c r="P56" s="50"/>
+      <c r="Q56" s="50"/>
+      <c r="R56" s="50"/>
+      <c r="S56" s="50"/>
+      <c r="T56" s="50"/>
+      <c r="U56" s="50"/>
+      <c r="V56" s="50"/>
+      <c r="W56" s="50"/>
+      <c r="X56" s="50"/>
+      <c r="Y56" s="50"/>
+      <c r="Z56" s="50"/>
+      <c r="AA56" s="50"/>
+    </row>
+    <row r="57" spans="1:27">
+      <c r="A57" s="50"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="50"/>
+      <c r="H57" s="50"/>
+      <c r="I57" s="50"/>
+      <c r="J57" s="50"/>
+      <c r="K57" s="50"/>
+      <c r="L57" s="50"/>
+      <c r="M57" s="50"/>
+      <c r="N57" s="50"/>
+      <c r="O57" s="50"/>
+      <c r="P57" s="50"/>
+      <c r="Q57" s="50"/>
+      <c r="R57" s="50"/>
+      <c r="S57" s="50"/>
+      <c r="T57" s="50"/>
+      <c r="U57" s="50"/>
+      <c r="V57" s="50"/>
+      <c r="W57" s="50"/>
+      <c r="X57" s="50"/>
+      <c r="Y57" s="50"/>
+      <c r="Z57" s="50"/>
+      <c r="AA57" s="50"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CB1F27-3E1D-1D4A-838D-AA35D1F874EF}">
+  <dimension ref="A1:AE57"/>
+  <sheetViews>
+    <sheetView topLeftCell="A20" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -734,7 +2433,7 @@
     <col min="29" max="29" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="17" thickBot="1">
+    <row r="1" spans="1:31" ht="17" thickBot="1">
       <c r="G1" t="s">
         <v>6</v>
       </c>
@@ -745,7 +2444,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:31">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -818,8 +2517,11 @@
       <c r="AC2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:29">
+      <c r="AE2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -875,7 +2577,7 @@
         <v>9</v>
       </c>
       <c r="W3" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>12</v>
@@ -895,8 +2597,11 @@
       <c r="AC3" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:29">
+      <c r="AE3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -961,7 +2666,7 @@
         <v>9</v>
       </c>
       <c r="Z4" s="34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA4" s="23" t="s">
         <v>13</v>
@@ -972,8 +2677,11 @@
       <c r="AC4" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:29">
+      <c r="AE4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1029,7 +2737,7 @@
         <v>9</v>
       </c>
       <c r="W5" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X5" s="5" t="s">
         <v>12</v>
@@ -1038,7 +2746,7 @@
         <v>9</v>
       </c>
       <c r="Z5" s="34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA5" s="23" t="s">
         <v>13</v>
@@ -1049,8 +2757,11 @@
       <c r="AC5" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:29">
+      <c r="AE5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1106,7 +2817,7 @@
         <v>9</v>
       </c>
       <c r="W6" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X6" s="16" t="s">
         <v>9</v>
@@ -1115,7 +2826,7 @@
         <v>9</v>
       </c>
       <c r="Z6" s="34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA6" s="23" t="s">
         <v>13</v>
@@ -1126,8 +2837,11 @@
       <c r="AC6" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:29">
+      <c r="AE6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1192,7 +2906,7 @@
         <v>9</v>
       </c>
       <c r="Z7" s="34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA7" s="23" t="s">
         <v>13</v>
@@ -1203,8 +2917,11 @@
       <c r="AC7" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:29">
+      <c r="AE7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1260,7 +2977,7 @@
         <v>9</v>
       </c>
       <c r="W8" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X8" s="5" t="s">
         <v>12</v>
@@ -1269,7 +2986,7 @@
         <v>9</v>
       </c>
       <c r="Z8" s="30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA8" s="25" t="s">
         <v>9</v>
@@ -1280,8 +2997,11 @@
       <c r="AC8" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:29">
+      <c r="AE8">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1337,7 +3057,7 @@
         <v>9</v>
       </c>
       <c r="W9" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X9" s="5" t="s">
         <v>12</v>
@@ -1346,7 +3066,7 @@
         <v>9</v>
       </c>
       <c r="Z9" s="30" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AA9" s="23" t="s">
         <v>13</v>
@@ -1357,8 +3077,11 @@
       <c r="AC9" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:29">
+      <c r="AE9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1414,7 +3137,7 @@
         <v>9</v>
       </c>
       <c r="W10" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X10" s="5" t="s">
         <v>12</v>
@@ -1434,8 +3157,11 @@
       <c r="AC10" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:29">
+      <c r="AE10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1491,7 +3217,7 @@
         <v>9</v>
       </c>
       <c r="W11" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X11" s="5" t="s">
         <v>12</v>
@@ -1500,7 +3226,7 @@
         <v>9</v>
       </c>
       <c r="Z11" s="30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA11" s="23" t="s">
         <v>13</v>
@@ -1511,8 +3237,11 @@
       <c r="AC11" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:29">
+      <c r="AE11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1577,7 +3306,7 @@
         <v>9</v>
       </c>
       <c r="Z12" s="34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA12" s="23" t="s">
         <v>13</v>
@@ -1588,8 +3317,11 @@
       <c r="AC12" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:29">
+      <c r="AE12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1654,7 +3386,7 @@
         <v>9</v>
       </c>
       <c r="Z13" s="34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA13" s="23" t="s">
         <v>13</v>
@@ -1665,8 +3397,11 @@
       <c r="AC13" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:29">
+      <c r="AE13">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1722,7 +3457,7 @@
         <v>9</v>
       </c>
       <c r="W14" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X14" s="5" t="s">
         <v>12</v>
@@ -1731,7 +3466,7 @@
         <v>9</v>
       </c>
       <c r="Z14" s="34" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AA14" s="23" t="s">
         <v>13</v>
@@ -1742,8 +3477,11 @@
       <c r="AC14" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:29">
+      <c r="AE14">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1799,7 +3537,7 @@
         <v>9</v>
       </c>
       <c r="W15" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X15" s="5" t="s">
         <v>12</v>
@@ -1819,8 +3557,11 @@
       <c r="AC15" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:29">
+      <c r="AE15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1876,7 +3617,7 @@
         <v>9</v>
       </c>
       <c r="W16" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X16" s="5" t="s">
         <v>12</v>
@@ -1896,8 +3637,11 @@
       <c r="AC16" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:29">
+      <c r="AE16">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1953,7 +3697,7 @@
         <v>9</v>
       </c>
       <c r="W17" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X17" s="5" t="s">
         <v>12</v>
@@ -1973,8 +3717,11 @@
       <c r="AC17" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" ht="44" customHeight="1">
+      <c r="AE17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" ht="44" customHeight="1">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2040,7 +3787,7 @@
         <v>9</v>
       </c>
       <c r="Z18" s="30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA18" s="25" t="s">
         <v>9</v>
@@ -2051,8 +3798,11 @@
       <c r="AC18" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:29">
+      <c r="AE18">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2117,7 +3867,7 @@
         <v>9</v>
       </c>
       <c r="Z19" s="30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA19" s="23" t="s">
         <v>13</v>
@@ -2128,8 +3878,11 @@
       <c r="AC19" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:29">
+      <c r="AE19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2185,7 +3938,7 @@
         <v>9</v>
       </c>
       <c r="W20" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X20" s="5" t="s">
         <v>12</v>
@@ -2194,7 +3947,7 @@
         <v>10</v>
       </c>
       <c r="Z20" s="34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA20" s="23" t="s">
         <v>13</v>
@@ -2205,8 +3958,11 @@
       <c r="AC20" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:29">
+      <c r="AE20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2262,7 +4018,7 @@
         <v>9</v>
       </c>
       <c r="W21" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X21" s="5" t="s">
         <v>12</v>
@@ -2271,7 +4027,7 @@
         <v>9</v>
       </c>
       <c r="Z21" s="34" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AA21" s="23" t="s">
         <v>13</v>
@@ -2282,8 +4038,11 @@
       <c r="AC21" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:29">
+      <c r="AE21">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -2348,7 +4107,7 @@
         <v>9</v>
       </c>
       <c r="Z22" s="34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA22" s="23" t="s">
         <v>13</v>
@@ -2359,8 +4118,11 @@
       <c r="AC22" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:29">
+      <c r="AE22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -2436,8 +4198,11 @@
       <c r="AC23" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:29">
+      <c r="AE23">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -2493,7 +4258,7 @@
         <v>9</v>
       </c>
       <c r="W24" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X24" s="5" t="s">
         <v>12</v>
@@ -2502,7 +4267,7 @@
         <v>9</v>
       </c>
       <c r="Z24" s="34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA24" s="23" t="s">
         <v>13</v>
@@ -2513,8 +4278,11 @@
       <c r="AC24" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:29">
+      <c r="AE24">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -2590,8 +4358,11 @@
       <c r="AC25" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:29">
+      <c r="AE25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -2647,7 +4418,7 @@
         <v>9</v>
       </c>
       <c r="W26" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X26" s="5" t="s">
         <v>12</v>
@@ -2656,7 +4427,7 @@
         <v>9</v>
       </c>
       <c r="Z26" s="30" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AA26" s="25" t="s">
         <v>9</v>
@@ -2667,8 +4438,11 @@
       <c r="AC26" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:29">
+      <c r="AE26">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -2724,7 +4498,7 @@
         <v>9</v>
       </c>
       <c r="W27" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X27" s="5" t="s">
         <v>12</v>
@@ -2744,8 +4518,11 @@
       <c r="AC27" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:29">
+      <c r="AE27">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -2801,7 +4578,7 @@
         <v>9</v>
       </c>
       <c r="W28" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X28" s="5" t="s">
         <v>12</v>
@@ -2821,8 +4598,11 @@
       <c r="AC28" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:29">
+      <c r="AE28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2878,7 +4658,7 @@
         <v>9</v>
       </c>
       <c r="W29" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X29" s="5" t="s">
         <v>12</v>
@@ -2887,7 +4667,7 @@
         <v>9</v>
       </c>
       <c r="Z29" s="34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AA29" s="23" t="s">
         <v>13</v>
@@ -2898,8 +4678,11 @@
       <c r="AC29" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:29">
+      <c r="AE29">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2975,8 +4758,11 @@
       <c r="AC30" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:29">
+      <c r="AE30">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -3032,7 +4818,7 @@
         <v>10</v>
       </c>
       <c r="W31" s="28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="X31" s="5" t="s">
         <v>12</v>
@@ -3041,7 +4827,7 @@
         <v>12</v>
       </c>
       <c r="Z31" s="30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AA31" s="25" t="s">
         <v>9</v>
@@ -3052,8 +4838,11 @@
       <c r="AC31" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:29">
+      <c r="AE31">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -3118,7 +4907,7 @@
         <v>9</v>
       </c>
       <c r="Z32" s="34" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AA32" s="23" t="s">
         <v>13</v>
@@ -3129,8 +4918,11 @@
       <c r="AC32" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:29">
+      <c r="AE32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -3195,7 +4987,7 @@
         <v>12</v>
       </c>
       <c r="Z33" s="30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AA33" s="23" t="s">
         <v>13</v>
@@ -3206,8 +4998,11 @@
       <c r="AC33" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:29">
+      <c r="AE33">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -3263,7 +5058,7 @@
         <v>9</v>
       </c>
       <c r="W34" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X34" s="5" t="s">
         <v>12</v>
@@ -3283,8 +5078,11 @@
       <c r="AC34" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:29">
+      <c r="AE34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -3360,8 +5158,11 @@
       <c r="AC35" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="1:29">
+      <c r="AE35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -3426,7 +5227,7 @@
         <v>11</v>
       </c>
       <c r="Z36" s="35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA36" s="22" t="s">
         <v>9</v>
@@ -3437,8 +5238,11 @@
       <c r="AC36" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:29">
+      <c r="AE36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -3494,7 +5298,7 @@
         <v>9</v>
       </c>
       <c r="W37" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X37" s="5" t="s">
         <v>12</v>
@@ -3514,8 +5318,11 @@
       <c r="AC37" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:29">
+      <c r="AE37">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -3571,7 +5378,7 @@
         <v>9</v>
       </c>
       <c r="W38" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X38" s="5" t="s">
         <v>12</v>
@@ -3580,7 +5387,7 @@
         <v>9</v>
       </c>
       <c r="Z38" s="34" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AA38" s="23" t="s">
         <v>13</v>
@@ -3591,8 +5398,11 @@
       <c r="AC38" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="1:29">
+      <c r="AE38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -3648,7 +5458,7 @@
         <v>9</v>
       </c>
       <c r="W39" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X39" s="5" t="s">
         <v>12</v>
@@ -3657,7 +5467,7 @@
         <v>9</v>
       </c>
       <c r="Z39" s="30" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AA39" s="25" t="s">
         <v>9</v>
@@ -3668,8 +5478,11 @@
       <c r="AC39" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="40" spans="1:29">
+      <c r="AE39">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -3725,7 +5538,7 @@
         <v>9</v>
       </c>
       <c r="W40" s="32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X40" s="5" t="s">
         <v>12</v>
@@ -3745,8 +5558,11 @@
       <c r="AC40" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:29" ht="17" thickBot="1">
+      <c r="AE40">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" ht="17" thickBot="1">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -3822,11 +5638,176 @@
       <c r="AC41" s="17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:29">
+      <c r="AE41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" ht="39">
+      <c r="A44" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="41"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+    </row>
+    <row r="45" spans="1:31" ht="39">
+      <c r="A45" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="41"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
       <c r="N45" t="s">
         <v>57</v>
       </c>
+    </row>
+    <row r="46" spans="1:31" ht="39">
+      <c r="A46" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+    </row>
+    <row r="47" spans="1:31" ht="39">
+      <c r="A47" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="41"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+    </row>
+    <row r="48" spans="1:31" ht="39">
+      <c r="A48" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="41"/>
+      <c r="C48" s="41"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
+      <c r="G48" s="41"/>
+      <c r="H48" s="41"/>
+      <c r="I48" s="41"/>
+    </row>
+    <row r="49" spans="1:9" ht="39">
+      <c r="A49" s="41"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
+    </row>
+    <row r="50" spans="1:9" ht="39">
+      <c r="A50" s="41"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="41"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="41"/>
+    </row>
+    <row r="51" spans="1:9" ht="39">
+      <c r="A51" s="41"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="41"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="41"/>
+    </row>
+    <row r="52" spans="1:9" ht="39">
+      <c r="A52" s="41"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="41"/>
+    </row>
+    <row r="53" spans="1:9" ht="39">
+      <c r="A53" s="41"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="41"/>
+    </row>
+    <row r="54" spans="1:9" ht="39">
+      <c r="A54" s="41"/>
+      <c r="B54" s="41"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="41"/>
+      <c r="H54" s="41"/>
+      <c r="I54" s="41"/>
+    </row>
+    <row r="55" spans="1:9" ht="39">
+      <c r="A55" s="41"/>
+      <c r="B55" s="41"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="41"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="41"/>
+      <c r="G55" s="41"/>
+      <c r="H55" s="41"/>
+      <c r="I55" s="41"/>
+    </row>
+    <row r="56" spans="1:9" ht="39">
+      <c r="A56" s="41"/>
+      <c r="B56" s="41"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="41"/>
+    </row>
+    <row r="57" spans="1:9" ht="39">
+      <c r="A57" s="41"/>
+      <c r="B57" s="41"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="41"/>
+      <c r="E57" s="41"/>
+      <c r="F57" s="41"/>
+      <c r="G57" s="41"/>
+      <c r="H57" s="41"/>
+      <c r="I57" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
exploring covariance structures of RE
</commit_message>
<xml_diff>
--- a/code/samples_summary_inference.xlsx
+++ b/code/samples_summary_inference.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morril01/Documents/PhD/GlobalDA/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9755E445-4CA6-E140-8DA0-6936092DA277}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3A4BEE-3EED-314C-A0E6-D4C146E6CEC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="2280" windowWidth="27640" windowHeight="16720" xr2:uid="{5DBFF44D-DF5C-A046-9A50-B35ED57F5618}"/>
+    <workbookView xWindow="1420" yWindow="460" windowWidth="27040" windowHeight="16720" xr2:uid="{5DBFF44D-DF5C-A046-9A50-B35ED57F5618}"/>
   </bookViews>
   <sheets>
     <sheet name="Full intercept" sheetId="4" r:id="rId1"/>
-    <sheet name="Single intercept" sheetId="1" r:id="rId2"/>
+    <sheet name="Uncorrelated (diagonal) interce" sheetId="5" r:id="rId2"/>
+    <sheet name="Single intercept" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1379" uniqueCount="70">
   <si>
     <t>nuc1 TMB</t>
   </si>
@@ -234,12 +235,15 @@
   <si>
     <t>Number of signatures</t>
   </si>
+  <si>
+    <t xml:space="preserve"> NA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -273,6 +277,29 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="120"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="7">
@@ -313,7 +340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -401,11 +428,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -457,6 +521,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,10 +934,10 @@
   <dimension ref="A1:AA57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="W35" sqref="W35"/>
+      <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="11.83203125" customWidth="1"/>
     <col min="12" max="12" width="13.1640625" customWidth="1"/>
@@ -792,7 +946,7 @@
     <col min="17" max="17" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="17" thickBot="1">
+    <row r="1" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>6</v>
       </c>
@@ -803,7 +957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -840,13 +994,13 @@
       <c r="Q2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="3" t="s">
         <v>65</v>
       </c>
       <c r="V2" t="s">
@@ -859,23 +1013,23 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="42"/>
       <c r="G3" s="43"/>
-      <c r="I3" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="42" t="s">
-        <v>12</v>
+      <c r="I3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="43"/>
@@ -883,14 +1037,17 @@
       <c r="O3" s="42"/>
       <c r="P3" s="16"/>
       <c r="Q3" s="43"/>
-      <c r="S3">
+      <c r="S3" s="10">
         <v>15</v>
       </c>
-      <c r="U3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="T3" s="58">
+        <v>19</v>
+      </c>
+      <c r="U3" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -902,10 +1059,10 @@
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="43"/>
-      <c r="I4" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="42" t="s">
+      <c r="I4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="5"/>
@@ -914,27 +1071,30 @@
       <c r="O4" s="42"/>
       <c r="P4" s="16"/>
       <c r="Q4" s="43"/>
-      <c r="S4">
-        <v>9</v>
-      </c>
-      <c r="U4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="S4" s="10">
+        <v>9</v>
+      </c>
+      <c r="T4" s="58">
+        <v>8</v>
+      </c>
+      <c r="U4" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="42" t="s">
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="42"/>
       <c r="G5" s="43"/>
-      <c r="I5" s="47" t="s">
-        <v>12</v>
+      <c r="I5" s="51" t="s">
+        <v>9</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>9</v>
@@ -945,29 +1105,32 @@
       <c r="O5" s="42"/>
       <c r="P5" s="16"/>
       <c r="Q5" s="43"/>
-      <c r="S5">
+      <c r="S5" s="10">
         <v>5</v>
       </c>
-      <c r="U5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="T5" s="58">
+        <v>6</v>
+      </c>
+      <c r="U5" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="43"/>
-      <c r="I6" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="42" t="s">
+      <c r="I6" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K6" s="5"/>
@@ -976,92 +1139,111 @@
       <c r="O6" s="42"/>
       <c r="P6" s="16"/>
       <c r="Q6" s="43"/>
-      <c r="S6">
-        <v>6</v>
-      </c>
-      <c r="U6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
-      <c r="A7" t="s">
+      <c r="S6" s="10">
+        <v>6</v>
+      </c>
+      <c r="T6" s="58">
+        <v>8</v>
+      </c>
+      <c r="U6" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="43"/>
-      <c r="I7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="43"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="42"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="43"/>
-      <c r="S7">
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="68"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="71"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="72"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="69"/>
+      <c r="R7" s="65"/>
+      <c r="S7" s="64">
         <v>27</v>
       </c>
-      <c r="U7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
-      <c r="A8" t="s">
+      <c r="T7" s="2">
+        <v>10</v>
+      </c>
+      <c r="U7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="43"/>
-      <c r="I8" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="43"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="43"/>
-      <c r="S8">
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="77"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="80"/>
+      <c r="L8" s="78"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="77"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="73">
         <v>136</v>
       </c>
-      <c r="U8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="T8" s="55">
+        <v>14</v>
+      </c>
+      <c r="U8" s="56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="42" t="s">
+      <c r="D9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="42"/>
       <c r="G9" s="43"/>
-      <c r="I9" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="42" t="s">
-        <v>12</v>
+      <c r="I9" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="43"/>
@@ -1069,14 +1251,17 @@
       <c r="O9" s="42"/>
       <c r="P9" s="16"/>
       <c r="Q9" s="43"/>
-      <c r="S9">
+      <c r="S9" s="10">
         <v>2</v>
       </c>
-      <c r="U9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="T9" s="58">
+        <v>67</v>
+      </c>
+      <c r="U9" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1088,10 +1273,10 @@
       </c>
       <c r="F10" s="42"/>
       <c r="G10" s="43"/>
-      <c r="I10" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="42" t="s">
+      <c r="I10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K10" s="5"/>
@@ -1100,18 +1285,21 @@
       <c r="O10" s="42"/>
       <c r="P10" s="16"/>
       <c r="Q10" s="43"/>
-      <c r="S10">
+      <c r="S10" s="10">
         <v>8</v>
       </c>
-      <c r="U10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="T10" s="58">
+        <v>6</v>
+      </c>
+      <c r="U10" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="6" t="s">
@@ -1119,10 +1307,10 @@
       </c>
       <c r="F11" s="42"/>
       <c r="G11" s="43"/>
-      <c r="I11" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="42" t="s">
+      <c r="I11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K11" s="5"/>
@@ -1131,29 +1319,32 @@
       <c r="O11" s="42"/>
       <c r="P11" s="16"/>
       <c r="Q11" s="43"/>
-      <c r="S11">
+      <c r="S11" s="10">
         <v>2</v>
       </c>
-      <c r="U11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="T11" s="58">
+        <v>4</v>
+      </c>
+      <c r="U11" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="42"/>
       <c r="G12" s="43"/>
-      <c r="I12" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="42" t="s">
+      <c r="I12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K12" s="5"/>
@@ -1162,76 +1353,95 @@
       <c r="O12" s="42"/>
       <c r="P12" s="16"/>
       <c r="Q12" s="43"/>
-      <c r="S12">
+      <c r="S12" s="10">
         <v>16</v>
       </c>
-      <c r="U12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24">
-      <c r="A13" t="s">
+      <c r="T12" s="58">
+        <v>7</v>
+      </c>
+      <c r="U12" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A13" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43"/>
-      <c r="I13" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="43"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="43"/>
-      <c r="S13">
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="68"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="71"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="65"/>
+      <c r="N13" s="72"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="68"/>
+      <c r="Q13" s="69"/>
+      <c r="R13" s="65"/>
+      <c r="S13" s="64">
         <v>34</v>
       </c>
-      <c r="U13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24">
-      <c r="A14" t="s">
+      <c r="T13" s="2">
+        <v>9</v>
+      </c>
+      <c r="U13" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="43"/>
-      <c r="I14" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="43"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="43"/>
-      <c r="S14">
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="83" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="77"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="79" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="80"/>
+      <c r="L14" s="78"/>
+      <c r="M14" s="74"/>
+      <c r="N14" s="81"/>
+      <c r="O14" s="77"/>
+      <c r="P14" s="77"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="74"/>
+      <c r="S14" s="73">
         <v>106</v>
       </c>
-      <c r="U14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24">
+      <c r="T14" s="55">
+        <v>9</v>
+      </c>
+      <c r="U14" s="56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1243,10 +1453,10 @@
       </c>
       <c r="F15" s="42"/>
       <c r="G15" s="43"/>
-      <c r="I15" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" s="42" t="s">
+      <c r="I15" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K15" s="5"/>
@@ -1255,278 +1465,344 @@
       <c r="O15" s="42"/>
       <c r="P15" s="16"/>
       <c r="Q15" s="43"/>
-      <c r="S15">
+      <c r="S15" s="10">
         <v>15</v>
       </c>
-      <c r="U15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24">
-      <c r="A16" t="s">
+      <c r="T15" s="58">
+        <v>6</v>
+      </c>
+      <c r="U15" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A16" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="43"/>
-      <c r="I16" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="43"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="43"/>
-      <c r="S16">
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="68"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="71"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="65"/>
+      <c r="N16" s="72"/>
+      <c r="O16" s="68"/>
+      <c r="P16" s="68"/>
+      <c r="Q16" s="69"/>
+      <c r="R16" s="65"/>
+      <c r="S16" s="64">
         <v>42</v>
       </c>
-      <c r="U16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
-      <c r="A17" t="s">
+      <c r="T16" s="2">
+        <v>7</v>
+      </c>
+      <c r="U16" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="43"/>
-      <c r="I17" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="43"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="43"/>
-      <c r="S17">
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="88"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="85"/>
+      <c r="I17" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="90"/>
+      <c r="L17" s="89"/>
+      <c r="M17" s="85"/>
+      <c r="N17" s="91"/>
+      <c r="O17" s="88"/>
+      <c r="P17" s="88"/>
+      <c r="Q17" s="89"/>
+      <c r="R17" s="85"/>
+      <c r="S17" s="84">
         <v>37</v>
       </c>
-      <c r="U17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="44" customHeight="1">
-      <c r="A18" t="s">
+      <c r="T17" s="58">
+        <v>9</v>
+      </c>
+      <c r="U17" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" s="52" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J18" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="43"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="43"/>
-      <c r="S18">
+      <c r="B18" s="93"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="94" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="96"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="99" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="100"/>
+      <c r="L18" s="97"/>
+      <c r="M18" s="93"/>
+      <c r="N18" s="101"/>
+      <c r="O18" s="96"/>
+      <c r="P18" s="96"/>
+      <c r="Q18" s="97"/>
+      <c r="R18" s="93"/>
+      <c r="S18" s="92">
         <v>65</v>
       </c>
-      <c r="U18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
-      <c r="A19" t="s">
+      <c r="T18" s="60">
+        <v>12</v>
+      </c>
+      <c r="U18" s="61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="42"/>
-      <c r="G19" s="43"/>
-      <c r="I19" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="K19" s="5"/>
-      <c r="L19" s="43"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="43"/>
-      <c r="S19">
+      <c r="B19" s="85"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="88"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="103" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="90"/>
+      <c r="L19" s="89"/>
+      <c r="M19" s="85"/>
+      <c r="N19" s="91"/>
+      <c r="O19" s="88"/>
+      <c r="P19" s="88"/>
+      <c r="Q19" s="89"/>
+      <c r="R19" s="85"/>
+      <c r="S19" s="84">
         <v>32</v>
       </c>
-      <c r="U19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
-      <c r="A20" t="s">
+      <c r="T19" s="58">
+        <v>12</v>
+      </c>
+      <c r="U19" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="42"/>
-      <c r="G20" s="43"/>
-      <c r="I20" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="K20" s="5"/>
-      <c r="L20" s="43"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="43"/>
-      <c r="S20">
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="88"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="103" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="90"/>
+      <c r="L20" s="89"/>
+      <c r="M20" s="85"/>
+      <c r="N20" s="91"/>
+      <c r="O20" s="88"/>
+      <c r="P20" s="88"/>
+      <c r="Q20" s="89"/>
+      <c r="R20" s="85"/>
+      <c r="S20" s="84">
         <v>38</v>
       </c>
-      <c r="U20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" t="s">
+      <c r="T20" s="58">
+        <v>8</v>
+      </c>
+      <c r="U20" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="43"/>
-      <c r="I21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K21" s="5"/>
-      <c r="L21" s="43"/>
-      <c r="N21" s="47"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="43"/>
-      <c r="S21">
+      <c r="B21" s="85"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="104" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="88"/>
+      <c r="G21" s="89"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="90"/>
+      <c r="L21" s="89"/>
+      <c r="M21" s="85"/>
+      <c r="N21" s="91"/>
+      <c r="O21" s="88"/>
+      <c r="P21" s="88"/>
+      <c r="Q21" s="89"/>
+      <c r="R21" s="85"/>
+      <c r="S21" s="84">
         <v>86</v>
       </c>
-      <c r="U21">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
-      <c r="A22" t="s">
+      <c r="T21" s="58">
+        <v>10</v>
+      </c>
+      <c r="U21" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="43"/>
-      <c r="I22" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J22" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K22" s="5"/>
-      <c r="L22" s="43"/>
-      <c r="N22" s="47"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="43"/>
-      <c r="S22">
+      <c r="B22" s="85"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="104" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="88"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="85"/>
+      <c r="I22" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="90"/>
+      <c r="L22" s="89"/>
+      <c r="M22" s="85"/>
+      <c r="N22" s="91"/>
+      <c r="O22" s="88"/>
+      <c r="P22" s="88"/>
+      <c r="Q22" s="89"/>
+      <c r="R22" s="85"/>
+      <c r="S22" s="84">
         <v>30</v>
       </c>
-      <c r="U22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
-      <c r="A23" t="s">
+      <c r="T22" s="58">
+        <v>10</v>
+      </c>
+      <c r="U22" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="42"/>
-      <c r="G23" s="43"/>
-      <c r="I23" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J23" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K23" s="5"/>
-      <c r="L23" s="43"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="43"/>
-      <c r="S23">
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="77"/>
+      <c r="G23" s="78"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="105" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="80"/>
+      <c r="L23" s="78"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="81"/>
+      <c r="O23" s="77"/>
+      <c r="P23" s="77"/>
+      <c r="Q23" s="78"/>
+      <c r="R23" s="74"/>
+      <c r="S23" s="73">
         <v>207</v>
       </c>
-      <c r="U23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
+      <c r="T23" s="55">
+        <v>18</v>
+      </c>
+      <c r="U23" s="56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="42"/>
       <c r="G24" s="43"/>
-      <c r="I24" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J24" s="42" t="s">
+      <c r="I24" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K24" s="5"/>
@@ -1535,111 +1811,138 @@
       <c r="O24" s="42"/>
       <c r="P24" s="16"/>
       <c r="Q24" s="43"/>
-      <c r="S24">
+      <c r="S24" s="10">
         <v>17</v>
       </c>
-      <c r="U24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
-      <c r="A25" t="s">
+      <c r="T24" s="58">
+        <v>12</v>
+      </c>
+      <c r="U24" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="42"/>
-      <c r="G25" s="43"/>
-      <c r="I25" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J25" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="K25" s="5"/>
-      <c r="L25" s="43"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="43"/>
-      <c r="S25">
+      <c r="B25" s="65"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="68"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="71"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="72"/>
+      <c r="O25" s="68"/>
+      <c r="P25" s="68"/>
+      <c r="Q25" s="69"/>
+      <c r="R25" s="65"/>
+      <c r="S25" s="64">
         <v>34</v>
       </c>
-      <c r="U25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
-      <c r="A26" t="s">
+      <c r="T25" s="2">
+        <v>7</v>
+      </c>
+      <c r="U25" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A26" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="42"/>
-      <c r="G26" s="43"/>
-      <c r="I26" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J26" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K26" s="5"/>
-      <c r="L26" s="43"/>
-      <c r="N26" s="47"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="43"/>
-      <c r="S26">
+      <c r="B26" s="85"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="88"/>
+      <c r="G26" s="89"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" s="90"/>
+      <c r="L26" s="89"/>
+      <c r="M26" s="85"/>
+      <c r="N26" s="91"/>
+      <c r="O26" s="88"/>
+      <c r="P26" s="88"/>
+      <c r="Q26" s="89"/>
+      <c r="R26" s="85"/>
+      <c r="S26" s="84">
         <v>51</v>
       </c>
-      <c r="U26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
-      <c r="A27" t="s">
+      <c r="T26" s="58">
+        <v>16</v>
+      </c>
+      <c r="U26" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="42"/>
-      <c r="G27" s="43"/>
-      <c r="I27" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J27" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K27" s="5"/>
-      <c r="L27" s="43"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="43"/>
-      <c r="S27">
+      <c r="B27" s="74"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="83" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="77"/>
+      <c r="G27" s="78"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="105" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="K27" s="80"/>
+      <c r="L27" s="78"/>
+      <c r="M27" s="74"/>
+      <c r="N27" s="81"/>
+      <c r="O27" s="77"/>
+      <c r="P27" s="77"/>
+      <c r="Q27" s="78"/>
+      <c r="R27" s="74"/>
+      <c r="S27" s="73">
         <v>53</v>
       </c>
-      <c r="U27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
+      <c r="T27" s="55">
+        <v>5</v>
+      </c>
+      <c r="U27" s="56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="6" t="s">
@@ -1647,7 +1950,7 @@
       </c>
       <c r="F28" s="42"/>
       <c r="G28" s="43"/>
-      <c r="I28" s="47" t="s">
+      <c r="I28" s="10" t="s">
         <v>10</v>
       </c>
       <c r="J28" s="6" t="s">
@@ -1659,18 +1962,21 @@
       <c r="O28" s="42"/>
       <c r="P28" s="16"/>
       <c r="Q28" s="43"/>
-      <c r="S28">
+      <c r="S28" s="10">
         <v>8</v>
       </c>
-      <c r="U28">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
+      <c r="T28" s="58">
+        <v>4</v>
+      </c>
+      <c r="U28" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D29" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="6" t="s">
@@ -1678,10 +1984,10 @@
       </c>
       <c r="F29" s="42"/>
       <c r="G29" s="43"/>
-      <c r="I29" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J29" s="42" t="s">
+      <c r="I29" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K29" s="5"/>
@@ -1690,138 +1996,173 @@
       <c r="O29" s="42"/>
       <c r="P29" s="16"/>
       <c r="Q29" s="43"/>
-      <c r="S29">
+      <c r="S29" s="10">
         <v>19</v>
       </c>
-      <c r="U29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21">
-      <c r="A30" t="s">
+      <c r="T29" s="58">
+        <v>6</v>
+      </c>
+      <c r="U29" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A30" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="42"/>
-      <c r="G30" s="43"/>
-      <c r="I30" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J30" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K30" s="5"/>
-      <c r="L30" s="43"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="43"/>
-      <c r="S30">
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="68"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="K30" s="71"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="65"/>
+      <c r="N30" s="72"/>
+      <c r="O30" s="68"/>
+      <c r="P30" s="68"/>
+      <c r="Q30" s="69"/>
+      <c r="R30" s="65"/>
+      <c r="S30" s="64">
         <v>97</v>
       </c>
-      <c r="U30">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
-      <c r="A31" t="s">
+      <c r="T30" s="2">
+        <v>13</v>
+      </c>
+      <c r="U30" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A31" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="42"/>
-      <c r="G31" s="43"/>
-      <c r="I31" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J31" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K31" s="5"/>
-      <c r="L31" s="43"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="43"/>
-      <c r="S31">
+      <c r="B31" s="85"/>
+      <c r="C31" s="85"/>
+      <c r="D31" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="88"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="85"/>
+      <c r="I31" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="K31" s="90"/>
+      <c r="L31" s="89"/>
+      <c r="M31" s="85"/>
+      <c r="N31" s="91"/>
+      <c r="O31" s="88"/>
+      <c r="P31" s="88"/>
+      <c r="Q31" s="89"/>
+      <c r="R31" s="85"/>
+      <c r="S31" s="84">
         <v>193</v>
       </c>
-      <c r="U31">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21">
-      <c r="A32" t="s">
+      <c r="T31" s="58">
+        <v>15</v>
+      </c>
+      <c r="U31" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A32" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="42"/>
-      <c r="G32" s="43"/>
-      <c r="I32" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J32" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="K32" s="5"/>
-      <c r="L32" s="43"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="43"/>
-      <c r="S32">
+      <c r="B32" s="85"/>
+      <c r="C32" s="85"/>
+      <c r="D32" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="88"/>
+      <c r="G32" s="89"/>
+      <c r="H32" s="85"/>
+      <c r="I32" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="K32" s="90"/>
+      <c r="L32" s="89"/>
+      <c r="M32" s="85"/>
+      <c r="N32" s="91"/>
+      <c r="O32" s="88"/>
+      <c r="P32" s="88"/>
+      <c r="Q32" s="89"/>
+      <c r="R32" s="85"/>
+      <c r="S32" s="84">
         <v>70</v>
       </c>
-      <c r="U32">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21">
-      <c r="A33" t="s">
+      <c r="T32" s="58">
+        <v>14</v>
+      </c>
+      <c r="U32" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="42"/>
-      <c r="G33" s="43"/>
-      <c r="I33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J33" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K33" s="5"/>
-      <c r="L33" s="43"/>
-      <c r="N33" s="47"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="43"/>
-      <c r="S33">
+      <c r="B33" s="74"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="105" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="77"/>
+      <c r="G33" s="78"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" s="77" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="80"/>
+      <c r="L33" s="78"/>
+      <c r="M33" s="74"/>
+      <c r="N33" s="81"/>
+      <c r="O33" s="77"/>
+      <c r="P33" s="77"/>
+      <c r="Q33" s="78"/>
+      <c r="R33" s="74"/>
+      <c r="S33" s="73">
         <v>208</v>
       </c>
-      <c r="U33">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21">
+      <c r="T33" s="55">
+        <v>17</v>
+      </c>
+      <c r="U33" s="56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -1833,10 +2174,10 @@
       </c>
       <c r="F34" s="42"/>
       <c r="G34" s="43"/>
-      <c r="I34" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J34" s="42" t="s">
+      <c r="I34" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J34" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K34" s="5"/>
@@ -1845,45 +2186,56 @@
       <c r="O34" s="42"/>
       <c r="P34" s="16"/>
       <c r="Q34" s="43"/>
-      <c r="S34">
+      <c r="S34" s="10">
         <v>15</v>
       </c>
-      <c r="U34">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21">
-      <c r="A35" t="s">
+      <c r="T34" s="58">
+        <v>9</v>
+      </c>
+      <c r="U34" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="42"/>
-      <c r="G35" s="43"/>
-      <c r="I35" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J35" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="K35" s="5"/>
-      <c r="L35" s="43"/>
-      <c r="N35" s="47"/>
-      <c r="O35" s="42"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="43"/>
-      <c r="S35">
+      <c r="B35" s="107"/>
+      <c r="C35" s="107"/>
+      <c r="D35" s="108" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="109" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="110"/>
+      <c r="G35" s="111"/>
+      <c r="H35" s="107"/>
+      <c r="I35" s="112" t="s">
+        <v>10</v>
+      </c>
+      <c r="J35" s="109" t="s">
+        <v>10</v>
+      </c>
+      <c r="K35" s="113"/>
+      <c r="L35" s="111"/>
+      <c r="M35" s="107"/>
+      <c r="N35" s="114"/>
+      <c r="O35" s="110"/>
+      <c r="P35" s="110"/>
+      <c r="Q35" s="111"/>
+      <c r="R35" s="107"/>
+      <c r="S35" s="106">
         <v>30</v>
       </c>
-      <c r="U35">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21">
+      <c r="T35" s="62">
+        <v>9</v>
+      </c>
+      <c r="U35" s="63">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -1923,29 +2275,32 @@
       <c r="Q36" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="S36" t="s">
+      <c r="S36" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="U36">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21">
+      <c r="T36" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="U36" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>49</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="42" t="s">
+      <c r="E37" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F37" s="42"/>
       <c r="G37" s="43"/>
-      <c r="I37" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J37" s="42" t="s">
+      <c r="I37" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J37" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K37" s="5"/>
@@ -1954,14 +2309,17 @@
       <c r="O37" s="42"/>
       <c r="P37" s="16"/>
       <c r="Q37" s="43"/>
-      <c r="S37">
+      <c r="S37" s="10">
         <v>15</v>
       </c>
-      <c r="U37">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21">
+      <c r="T37" s="58">
+        <v>7</v>
+      </c>
+      <c r="U37" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -1973,10 +2331,10 @@
       </c>
       <c r="F38" s="42"/>
       <c r="G38" s="43"/>
-      <c r="I38" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J38" s="42" t="s">
+      <c r="I38" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J38" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K38" s="5"/>
@@ -1985,107 +2343,134 @@
       <c r="O38" s="42"/>
       <c r="P38" s="16"/>
       <c r="Q38" s="43"/>
-      <c r="S38">
+      <c r="S38" s="10">
         <v>15</v>
       </c>
-      <c r="U38">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21">
-      <c r="A39" t="s">
+      <c r="T38" s="58">
+        <v>8</v>
+      </c>
+      <c r="U38" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A39" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="42"/>
-      <c r="G39" s="43"/>
-      <c r="I39" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="J39" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="K39" s="5"/>
-      <c r="L39" s="43"/>
-      <c r="N39" s="47"/>
-      <c r="O39" s="42"/>
-      <c r="P39" s="16"/>
-      <c r="Q39" s="43"/>
-      <c r="S39">
+      <c r="B39" s="65"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="68"/>
+      <c r="G39" s="69"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="J39" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="K39" s="71"/>
+      <c r="L39" s="69"/>
+      <c r="M39" s="65"/>
+      <c r="N39" s="72"/>
+      <c r="O39" s="68"/>
+      <c r="P39" s="68"/>
+      <c r="Q39" s="69"/>
+      <c r="R39" s="65"/>
+      <c r="S39" s="64">
         <v>30</v>
       </c>
-      <c r="U39">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21">
-      <c r="A40" t="s">
+      <c r="T39" s="2">
+        <v>17</v>
+      </c>
+      <c r="U39" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A40" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="42"/>
-      <c r="G40" s="43"/>
-      <c r="I40" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="J40" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="K40" s="5"/>
-      <c r="L40" s="43"/>
-      <c r="N40" s="47"/>
-      <c r="O40" s="42"/>
-      <c r="P40" s="16"/>
-      <c r="Q40" s="43"/>
-      <c r="S40">
+      <c r="B40" s="85"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="104" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="88"/>
+      <c r="G40" s="89"/>
+      <c r="H40" s="85"/>
+      <c r="I40" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="K40" s="90"/>
+      <c r="L40" s="89"/>
+      <c r="M40" s="85"/>
+      <c r="N40" s="91"/>
+      <c r="O40" s="88"/>
+      <c r="P40" s="88"/>
+      <c r="Q40" s="89"/>
+      <c r="R40" s="85"/>
+      <c r="S40" s="84">
         <v>41</v>
       </c>
-      <c r="U40">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" ht="17" thickBot="1">
-      <c r="A41" t="s">
+      <c r="T40" s="58">
+        <v>7</v>
+      </c>
+      <c r="U40" s="59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="45"/>
-      <c r="G41" s="46"/>
-      <c r="I41" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="J41" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="K41" s="12"/>
-      <c r="L41" s="46"/>
-      <c r="N41" s="48"/>
-      <c r="O41" s="45"/>
-      <c r="P41" s="44"/>
-      <c r="Q41" s="46"/>
-      <c r="S41">
+      <c r="B41" s="74"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="77"/>
+      <c r="G41" s="78"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="105" t="s">
+        <v>10</v>
+      </c>
+      <c r="J41" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="K41" s="80"/>
+      <c r="L41" s="78"/>
+      <c r="M41" s="74"/>
+      <c r="N41" s="81"/>
+      <c r="O41" s="77"/>
+      <c r="P41" s="77"/>
+      <c r="Q41" s="78"/>
+      <c r="R41" s="74"/>
+      <c r="S41" s="73">
         <v>40</v>
       </c>
-      <c r="U41">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="26">
+      <c r="T41" s="55">
+        <v>11</v>
+      </c>
+      <c r="U41" s="56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="26" x14ac:dyDescent="0.3">
       <c r="A44" s="49" t="s">
         <v>62</v>
       </c>
@@ -2098,7 +2483,7 @@
       <c r="H44" s="49"/>
       <c r="I44" s="49"/>
     </row>
-    <row r="45" spans="1:21" ht="26">
+    <row r="45" spans="1:21" ht="26" x14ac:dyDescent="0.3">
       <c r="A45" s="49" t="s">
         <v>61</v>
       </c>
@@ -2111,7 +2496,7 @@
       <c r="H45" s="49"/>
       <c r="I45" s="49"/>
     </row>
-    <row r="46" spans="1:21" ht="26">
+    <row r="46" spans="1:21" ht="26" x14ac:dyDescent="0.3">
       <c r="A46" s="49" t="s">
         <v>60</v>
       </c>
@@ -2124,7 +2509,7 @@
       <c r="H46" s="49"/>
       <c r="I46" s="49"/>
     </row>
-    <row r="47" spans="1:21" ht="26">
+    <row r="47" spans="1:21" ht="26" x14ac:dyDescent="0.3">
       <c r="A47" s="49" t="s">
         <v>64</v>
       </c>
@@ -2137,7 +2522,7 @@
       <c r="H47" s="49"/>
       <c r="I47" s="49"/>
     </row>
-    <row r="48" spans="1:21" ht="26">
+    <row r="48" spans="1:21" ht="26" x14ac:dyDescent="0.3">
       <c r="A48" s="49" t="s">
         <v>63</v>
       </c>
@@ -2150,7 +2535,7 @@
       <c r="H48" s="49"/>
       <c r="I48" s="49"/>
     </row>
-    <row r="49" spans="1:27">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49" s="50"/>
       <c r="B49" s="50"/>
       <c r="C49" s="50"/>
@@ -2179,7 +2564,7 @@
       <c r="Z49" s="50"/>
       <c r="AA49" s="50"/>
     </row>
-    <row r="50" spans="1:27">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50" s="50"/>
       <c r="B50" s="50"/>
       <c r="C50" s="50"/>
@@ -2208,7 +2593,7 @@
       <c r="Z50" s="50"/>
       <c r="AA50" s="50"/>
     </row>
-    <row r="51" spans="1:27">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A51" s="50"/>
       <c r="B51" s="50"/>
       <c r="C51" s="50"/>
@@ -2237,7 +2622,7 @@
       <c r="Z51" s="50"/>
       <c r="AA51" s="50"/>
     </row>
-    <row r="52" spans="1:27">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A52" s="50"/>
       <c r="B52" s="50"/>
       <c r="C52" s="50"/>
@@ -2266,7 +2651,7 @@
       <c r="Z52" s="50"/>
       <c r="AA52" s="50"/>
     </row>
-    <row r="53" spans="1:27">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A53" s="50"/>
       <c r="B53" s="50"/>
       <c r="C53" s="50"/>
@@ -2295,7 +2680,7 @@
       <c r="Z53" s="50"/>
       <c r="AA53" s="50"/>
     </row>
-    <row r="54" spans="1:27">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A54" s="50"/>
       <c r="B54" s="50"/>
       <c r="C54" s="50"/>
@@ -2324,7 +2709,7 @@
       <c r="Z54" s="50"/>
       <c r="AA54" s="50"/>
     </row>
-    <row r="55" spans="1:27">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A55" s="50"/>
       <c r="B55" s="50"/>
       <c r="C55" s="50"/>
@@ -2353,7 +2738,7 @@
       <c r="Z55" s="50"/>
       <c r="AA55" s="50"/>
     </row>
-    <row r="56" spans="1:27">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A56" s="50"/>
       <c r="B56" s="50"/>
       <c r="C56" s="50"/>
@@ -2382,7 +2767,7 @@
       <c r="Z56" s="50"/>
       <c r="AA56" s="50"/>
     </row>
-    <row r="57" spans="1:27">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A57" s="50"/>
       <c r="B57" s="50"/>
       <c r="C57" s="50"/>
@@ -2417,14 +2802,1648 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD28245-3C05-974D-A2D5-2DA00269A297}">
+  <dimension ref="A1:Y47"/>
+  <sheetViews>
+    <sheetView zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" t="s">
+        <v>58</v>
+      </c>
+      <c r="T2" t="s">
+        <v>68</v>
+      </c>
+      <c r="U2" t="s">
+        <v>65</v>
+      </c>
+      <c r="V2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W2" t="s">
+        <v>67</v>
+      </c>
+      <c r="X2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53">
+        <v>15</v>
+      </c>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53">
+        <v>6</v>
+      </c>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53"/>
+      <c r="X3" s="53"/>
+      <c r="Y3" s="53"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="53"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="53">
+        <v>9</v>
+      </c>
+      <c r="T4" s="53"/>
+      <c r="U4" s="53">
+        <v>6</v>
+      </c>
+      <c r="V4" s="53"/>
+      <c r="W4" s="53"/>
+      <c r="X4" s="53"/>
+      <c r="Y4" s="53"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="53"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53">
+        <v>5</v>
+      </c>
+      <c r="T5" s="53"/>
+      <c r="U5" s="53">
+        <v>6</v>
+      </c>
+      <c r="V5" s="53"/>
+      <c r="W5" s="53"/>
+      <c r="X5" s="53"/>
+      <c r="Y5" s="53"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="53"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="53">
+        <v>6</v>
+      </c>
+      <c r="T6" s="53"/>
+      <c r="U6" s="53">
+        <v>6</v>
+      </c>
+      <c r="V6" s="53"/>
+      <c r="W6" s="53"/>
+      <c r="X6" s="53"/>
+      <c r="Y6" s="53"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="53"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="53"/>
+      <c r="S7" s="53">
+        <v>27</v>
+      </c>
+      <c r="T7" s="53"/>
+      <c r="U7" s="53">
+        <v>6</v>
+      </c>
+      <c r="V7" s="53"/>
+      <c r="W7" s="53"/>
+      <c r="X7" s="53"/>
+      <c r="Y7" s="53"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="53"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="53">
+        <v>136</v>
+      </c>
+      <c r="T8" s="53"/>
+      <c r="U8" s="53">
+        <v>6</v>
+      </c>
+      <c r="V8" s="53"/>
+      <c r="W8" s="53"/>
+      <c r="X8" s="53"/>
+      <c r="Y8" s="53"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="53"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="53"/>
+      <c r="S9" s="53">
+        <v>2</v>
+      </c>
+      <c r="T9" s="53"/>
+      <c r="U9" s="53">
+        <v>6</v>
+      </c>
+      <c r="V9" s="53"/>
+      <c r="W9" s="53"/>
+      <c r="X9" s="53"/>
+      <c r="Y9" s="53"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="53"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="53"/>
+      <c r="S10" s="53">
+        <v>8</v>
+      </c>
+      <c r="T10" s="53"/>
+      <c r="U10" s="53">
+        <v>6</v>
+      </c>
+      <c r="V10" s="53"/>
+      <c r="W10" s="53"/>
+      <c r="X10" s="53"/>
+      <c r="Y10" s="53"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="53"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="53">
+        <v>2</v>
+      </c>
+      <c r="T11" s="53"/>
+      <c r="U11" s="53">
+        <v>6</v>
+      </c>
+      <c r="V11" s="53"/>
+      <c r="W11" s="53"/>
+      <c r="X11" s="53"/>
+      <c r="Y11" s="53"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="53"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="53"/>
+      <c r="S12" s="53">
+        <v>16</v>
+      </c>
+      <c r="T12" s="53"/>
+      <c r="U12" s="53">
+        <v>6</v>
+      </c>
+      <c r="V12" s="53"/>
+      <c r="W12" s="53"/>
+      <c r="X12" s="53"/>
+      <c r="Y12" s="53"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="53"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="42"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="53">
+        <v>34</v>
+      </c>
+      <c r="T13" s="53"/>
+      <c r="U13" s="53">
+        <v>6</v>
+      </c>
+      <c r="V13" s="53"/>
+      <c r="W13" s="53"/>
+      <c r="X13" s="53"/>
+      <c r="Y13" s="53"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="53"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="53"/>
+      <c r="S14" s="53">
+        <v>106</v>
+      </c>
+      <c r="T14" s="53"/>
+      <c r="U14" s="53">
+        <v>6</v>
+      </c>
+      <c r="V14" s="53"/>
+      <c r="W14" s="53"/>
+      <c r="X14" s="53"/>
+      <c r="Y14" s="53"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="53"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="53"/>
+      <c r="S15" s="53">
+        <v>15</v>
+      </c>
+      <c r="T15" s="53"/>
+      <c r="U15" s="53">
+        <v>6</v>
+      </c>
+      <c r="V15" s="53"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="53"/>
+      <c r="Y15" s="53"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="53"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="53"/>
+      <c r="S16" s="53">
+        <v>42</v>
+      </c>
+      <c r="T16" s="53"/>
+      <c r="U16" s="53">
+        <v>6</v>
+      </c>
+      <c r="V16" s="53"/>
+      <c r="W16" s="53"/>
+      <c r="X16" s="53"/>
+      <c r="Y16" s="53"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="53"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="42"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="53"/>
+      <c r="S17" s="53">
+        <v>37</v>
+      </c>
+      <c r="T17" s="53"/>
+      <c r="U17" s="53">
+        <v>6</v>
+      </c>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="53"/>
+      <c r="Y17" s="53"/>
+    </row>
+    <row r="18" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="1.65">
+      <c r="A18" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="53"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="5"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="42"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="43"/>
+      <c r="R18" s="53"/>
+      <c r="S18" s="53">
+        <v>65</v>
+      </c>
+      <c r="T18" s="53"/>
+      <c r="U18" s="53">
+        <v>6</v>
+      </c>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="53"/>
+      <c r="Y18" s="53"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="53"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="53"/>
+      <c r="S19" s="53">
+        <v>32</v>
+      </c>
+      <c r="T19" s="53"/>
+      <c r="U19" s="53">
+        <v>6</v>
+      </c>
+      <c r="V19" s="53"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="53"/>
+      <c r="Y19" s="53"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="53"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="53"/>
+      <c r="S20" s="53">
+        <v>38</v>
+      </c>
+      <c r="T20" s="53"/>
+      <c r="U20" s="53">
+        <v>6</v>
+      </c>
+      <c r="V20" s="53"/>
+      <c r="W20" s="53"/>
+      <c r="X20" s="53"/>
+      <c r="Y20" s="53"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="53"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="53"/>
+      <c r="S21" s="53">
+        <v>86</v>
+      </c>
+      <c r="T21" s="53"/>
+      <c r="U21" s="53">
+        <v>6</v>
+      </c>
+      <c r="V21" s="53"/>
+      <c r="W21" s="53"/>
+      <c r="X21" s="53"/>
+      <c r="Y21" s="53"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="53"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="53"/>
+      <c r="S22" s="53">
+        <v>30</v>
+      </c>
+      <c r="T22" s="53"/>
+      <c r="U22" s="53">
+        <v>6</v>
+      </c>
+      <c r="V22" s="53"/>
+      <c r="W22" s="53"/>
+      <c r="X22" s="53"/>
+      <c r="Y22" s="53"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="53"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="53"/>
+      <c r="S23" s="53">
+        <v>207</v>
+      </c>
+      <c r="T23" s="53"/>
+      <c r="U23" s="53">
+        <v>6</v>
+      </c>
+      <c r="V23" s="53"/>
+      <c r="W23" s="53"/>
+      <c r="X23" s="53"/>
+      <c r="Y23" s="53"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="53"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="53">
+        <v>17</v>
+      </c>
+      <c r="T24" s="53"/>
+      <c r="U24" s="53">
+        <v>6</v>
+      </c>
+      <c r="V24" s="53"/>
+      <c r="W24" s="53"/>
+      <c r="X24" s="53"/>
+      <c r="Y24" s="53"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="53"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="5"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="53"/>
+      <c r="S25" s="53">
+        <v>34</v>
+      </c>
+      <c r="T25" s="53"/>
+      <c r="U25" s="53">
+        <v>6</v>
+      </c>
+      <c r="V25" s="53"/>
+      <c r="W25" s="53"/>
+      <c r="X25" s="53"/>
+      <c r="Y25" s="53"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="53"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="5"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="53"/>
+      <c r="S26" s="53">
+        <v>51</v>
+      </c>
+      <c r="T26" s="53"/>
+      <c r="U26" s="53">
+        <v>6</v>
+      </c>
+      <c r="V26" s="53"/>
+      <c r="W26" s="53"/>
+      <c r="X26" s="53"/>
+      <c r="Y26" s="53"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="53"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K27" s="5"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="53"/>
+      <c r="S27" s="53">
+        <v>53</v>
+      </c>
+      <c r="T27" s="53"/>
+      <c r="U27" s="53">
+        <v>6</v>
+      </c>
+      <c r="V27" s="53"/>
+      <c r="W27" s="53"/>
+      <c r="X27" s="53"/>
+      <c r="Y27" s="53"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="53"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J28" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K28" s="5"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="53"/>
+      <c r="S28" s="53">
+        <v>8</v>
+      </c>
+      <c r="T28" s="53"/>
+      <c r="U28" s="53">
+        <v>6</v>
+      </c>
+      <c r="V28" s="53"/>
+      <c r="W28" s="53"/>
+      <c r="X28" s="53"/>
+      <c r="Y28" s="53"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="53"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" s="5"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="53"/>
+      <c r="S29" s="53">
+        <v>19</v>
+      </c>
+      <c r="T29" s="53"/>
+      <c r="U29" s="53">
+        <v>6</v>
+      </c>
+      <c r="V29" s="53"/>
+      <c r="W29" s="53"/>
+      <c r="X29" s="53"/>
+      <c r="Y29" s="53"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="53"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K30" s="5"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="53"/>
+      <c r="N30" s="47"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="53"/>
+      <c r="S30" s="53">
+        <v>97</v>
+      </c>
+      <c r="T30" s="53"/>
+      <c r="U30" s="53">
+        <v>6</v>
+      </c>
+      <c r="V30" s="53"/>
+      <c r="W30" s="53"/>
+      <c r="X30" s="53"/>
+      <c r="Y30" s="53"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="53"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K31" s="5"/>
+      <c r="L31" s="43"/>
+      <c r="M31" s="53"/>
+      <c r="N31" s="47"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="53"/>
+      <c r="S31" s="53">
+        <v>193</v>
+      </c>
+      <c r="T31" s="53"/>
+      <c r="U31" s="53">
+        <v>6</v>
+      </c>
+      <c r="V31" s="53"/>
+      <c r="W31" s="53"/>
+      <c r="X31" s="53"/>
+      <c r="Y31" s="53"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="53"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K32" s="5"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="53"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="53"/>
+      <c r="S32" s="53">
+        <v>70</v>
+      </c>
+      <c r="T32" s="53"/>
+      <c r="U32" s="53">
+        <v>6</v>
+      </c>
+      <c r="V32" s="53"/>
+      <c r="W32" s="53"/>
+      <c r="X32" s="53"/>
+      <c r="Y32" s="53"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="53"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J33" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="5"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="53"/>
+      <c r="N33" s="47"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="53"/>
+      <c r="S33" s="53">
+        <v>208</v>
+      </c>
+      <c r="T33" s="53"/>
+      <c r="U33" s="53">
+        <v>6</v>
+      </c>
+      <c r="V33" s="53"/>
+      <c r="W33" s="53"/>
+      <c r="X33" s="53"/>
+      <c r="Y33" s="53"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="53"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="J34" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K34" s="5"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="53"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="43"/>
+      <c r="R34" s="53"/>
+      <c r="S34" s="53">
+        <v>15</v>
+      </c>
+      <c r="T34" s="53"/>
+      <c r="U34" s="53">
+        <v>6</v>
+      </c>
+      <c r="V34" s="53"/>
+      <c r="W34" s="53"/>
+      <c r="X34" s="53"/>
+      <c r="Y34" s="53"/>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="53"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J35" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K35" s="5"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="53"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="43"/>
+      <c r="R35" s="53"/>
+      <c r="S35" s="53">
+        <v>30</v>
+      </c>
+      <c r="T35" s="53"/>
+      <c r="U35" s="53">
+        <v>6</v>
+      </c>
+      <c r="V35" s="53"/>
+      <c r="W35" s="53"/>
+      <c r="X35" s="53"/>
+      <c r="Y35" s="53"/>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="53"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="19"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="53"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="53"/>
+      <c r="S36" s="53"/>
+      <c r="T36" s="53"/>
+      <c r="U36" s="53">
+        <v>6</v>
+      </c>
+      <c r="V36" s="53"/>
+      <c r="W36" s="53"/>
+      <c r="X36" s="53"/>
+      <c r="Y36" s="53"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="53"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J37" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K37" s="5"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="53"/>
+      <c r="N37" s="47"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="43"/>
+      <c r="R37" s="53"/>
+      <c r="S37" s="53">
+        <v>15</v>
+      </c>
+      <c r="T37" s="53"/>
+      <c r="U37" s="53">
+        <v>6</v>
+      </c>
+      <c r="V37" s="53"/>
+      <c r="W37" s="53"/>
+      <c r="X37" s="53"/>
+      <c r="Y37" s="53"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="53"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="J38" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K38" s="5"/>
+      <c r="L38" s="43"/>
+      <c r="M38" s="53"/>
+      <c r="N38" s="47"/>
+      <c r="O38" s="42"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="43"/>
+      <c r="R38" s="53"/>
+      <c r="S38" s="53">
+        <v>15</v>
+      </c>
+      <c r="T38" s="53"/>
+      <c r="U38" s="53">
+        <v>6</v>
+      </c>
+      <c r="V38" s="53"/>
+      <c r="W38" s="53"/>
+      <c r="X38" s="53"/>
+      <c r="Y38" s="53"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="53"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J39" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K39" s="5"/>
+      <c r="L39" s="43"/>
+      <c r="M39" s="53"/>
+      <c r="N39" s="47"/>
+      <c r="O39" s="42"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="43"/>
+      <c r="R39" s="53"/>
+      <c r="S39" s="53">
+        <v>30</v>
+      </c>
+      <c r="T39" s="53"/>
+      <c r="U39" s="53">
+        <v>6</v>
+      </c>
+      <c r="V39" s="53"/>
+      <c r="W39" s="53"/>
+      <c r="X39" s="53"/>
+      <c r="Y39" s="53"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="53"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K40" s="5"/>
+      <c r="L40" s="43"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="47"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="16"/>
+      <c r="Q40" s="43"/>
+      <c r="R40" s="53"/>
+      <c r="S40" s="53">
+        <v>41</v>
+      </c>
+      <c r="T40" s="53"/>
+      <c r="U40" s="53">
+        <v>6</v>
+      </c>
+      <c r="V40" s="53"/>
+      <c r="W40" s="53"/>
+      <c r="X40" s="53"/>
+      <c r="Y40" s="53"/>
+    </row>
+    <row r="41" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="53"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="J41" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="K41" s="12"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="53"/>
+      <c r="N41" s="48"/>
+      <c r="O41" s="45"/>
+      <c r="P41" s="44"/>
+      <c r="Q41" s="46"/>
+      <c r="R41" s="53"/>
+      <c r="S41" s="53">
+        <v>40</v>
+      </c>
+      <c r="T41" s="53"/>
+      <c r="U41" s="53">
+        <v>6</v>
+      </c>
+      <c r="V41" s="53"/>
+      <c r="W41" s="53"/>
+      <c r="X41" s="53"/>
+      <c r="Y41" s="53"/>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="53"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="53"/>
+      <c r="R42" s="53"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
+      <c r="U42" s="53"/>
+      <c r="V42" s="53"/>
+      <c r="W42" s="53"/>
+      <c r="X42" s="53"/>
+      <c r="Y42" s="53"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="53"/>
+      <c r="K43" s="53"/>
+      <c r="L43" s="53"/>
+      <c r="M43" s="53"/>
+      <c r="N43" s="53"/>
+      <c r="O43" s="53"/>
+      <c r="P43" s="53"/>
+      <c r="Q43" s="53"/>
+      <c r="R43" s="53"/>
+      <c r="S43" s="53"/>
+      <c r="T43" s="53"/>
+      <c r="U43" s="53"/>
+      <c r="V43" s="53"/>
+      <c r="W43" s="53"/>
+      <c r="X43" s="53"/>
+      <c r="Y43" s="53"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
+      <c r="K44" s="53"/>
+      <c r="L44" s="53"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="53"/>
+      <c r="O44" s="53"/>
+      <c r="P44" s="53"/>
+      <c r="Q44" s="53"/>
+      <c r="R44" s="53"/>
+      <c r="S44" s="53"/>
+      <c r="T44" s="53"/>
+      <c r="U44" s="53"/>
+      <c r="V44" s="53"/>
+      <c r="W44" s="53"/>
+      <c r="X44" s="53"/>
+      <c r="Y44" s="53"/>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
+      <c r="K45" s="53"/>
+      <c r="L45" s="53"/>
+      <c r="M45" s="53"/>
+      <c r="N45" s="53"/>
+      <c r="O45" s="53"/>
+      <c r="P45" s="53"/>
+      <c r="Q45" s="53"/>
+      <c r="R45" s="53"/>
+      <c r="S45" s="53"/>
+      <c r="T45" s="53"/>
+      <c r="U45" s="53"/>
+      <c r="V45" s="53"/>
+      <c r="W45" s="53"/>
+      <c r="X45" s="53"/>
+      <c r="Y45" s="53"/>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
+      <c r="K46" s="53"/>
+      <c r="L46" s="53"/>
+      <c r="M46" s="53"/>
+      <c r="N46" s="53"/>
+      <c r="O46" s="53"/>
+      <c r="P46" s="53"/>
+      <c r="Q46" s="53"/>
+      <c r="R46" s="53"/>
+      <c r="S46" s="53"/>
+      <c r="T46" s="53"/>
+      <c r="U46" s="53"/>
+      <c r="V46" s="53"/>
+      <c r="W46" s="53"/>
+      <c r="X46" s="53"/>
+      <c r="Y46" s="53"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="53"/>
+      <c r="J47" s="53"/>
+      <c r="K47" s="53"/>
+      <c r="L47" s="53"/>
+      <c r="M47" s="53"/>
+      <c r="N47" s="53"/>
+      <c r="O47" s="53"/>
+      <c r="P47" s="53"/>
+      <c r="Q47" s="53"/>
+      <c r="R47" s="53"/>
+      <c r="S47" s="53"/>
+      <c r="T47" s="53"/>
+      <c r="U47" s="53"/>
+      <c r="V47" s="53"/>
+      <c r="W47" s="53"/>
+      <c r="X47" s="53"/>
+      <c r="Y47" s="53"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7CB1F27-3E1D-1D4A-838D-AA35D1F874EF}">
   <dimension ref="A1:AE57"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="Z18" sqref="Z18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="11" max="11" width="19" customWidth="1"/>
     <col min="20" max="20" width="19.6640625" customWidth="1"/>
@@ -2433,7 +4452,7 @@
     <col min="29" max="29" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="17" thickBot="1">
+    <row r="1" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
         <v>6</v>
       </c>
@@ -2444,7 +4463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2521,7 +4540,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2601,7 +4620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2681,7 +4700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2761,7 +4780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2841,7 +4860,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2921,7 +4940,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -3001,7 +5020,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -3081,7 +5100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -3161,7 +5180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -3241,7 +5260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3321,7 +5340,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -3401,7 +5420,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -3481,7 +5500,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -3561,7 +5580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -3641,7 +5660,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -3721,8 +5740,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="44" customHeight="1">
-      <c r="A18" t="s">
+    <row r="18" spans="1:31" ht="20" customHeight="1" x14ac:dyDescent="1.65">
+      <c r="A18" s="52" t="s">
         <v>31</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -3802,7 +5821,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -3882,7 +5901,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -3962,7 +5981,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -4042,7 +6061,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -4122,7 +6141,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -4202,7 +6221,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -4282,7 +6301,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -4362,7 +6381,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -4442,7 +6461,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -4522,7 +6541,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -4602,7 +6621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -4682,7 +6701,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -4762,7 +6781,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -4842,7 +6861,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -4922,7 +6941,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -5002,7 +7021,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -5082,7 +7101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -5162,7 +7181,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -5242,7 +7261,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -5322,7 +7341,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -5402,7 +7421,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -5482,7 +7501,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -5562,7 +7581,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="1:31" ht="17" thickBot="1">
+    <row r="41" spans="1:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -5642,7 +7661,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:31" ht="39">
+    <row r="44" spans="1:31" ht="39" x14ac:dyDescent="0.45">
       <c r="A44" s="41" t="s">
         <v>62</v>
       </c>
@@ -5655,7 +7674,7 @@
       <c r="H44" s="41"/>
       <c r="I44" s="41"/>
     </row>
-    <row r="45" spans="1:31" ht="39">
+    <row r="45" spans="1:31" ht="39" x14ac:dyDescent="0.45">
       <c r="A45" s="41" t="s">
         <v>61</v>
       </c>
@@ -5671,7 +7690,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:31" ht="39">
+    <row r="46" spans="1:31" ht="39" x14ac:dyDescent="0.45">
       <c r="A46" s="41" t="s">
         <v>60</v>
       </c>
@@ -5684,7 +7703,7 @@
       <c r="H46" s="41"/>
       <c r="I46" s="41"/>
     </row>
-    <row r="47" spans="1:31" ht="39">
+    <row r="47" spans="1:31" ht="39" x14ac:dyDescent="0.45">
       <c r="A47" s="41" t="s">
         <v>64</v>
       </c>
@@ -5697,7 +7716,7 @@
       <c r="H47" s="41"/>
       <c r="I47" s="41"/>
     </row>
-    <row r="48" spans="1:31" ht="39">
+    <row r="48" spans="1:31" ht="39" x14ac:dyDescent="0.45">
       <c r="A48" s="41" t="s">
         <v>63</v>
       </c>
@@ -5710,7 +7729,7 @@
       <c r="H48" s="41"/>
       <c r="I48" s="41"/>
     </row>
-    <row r="49" spans="1:9" ht="39">
+    <row r="49" spans="1:9" ht="39" x14ac:dyDescent="0.45">
       <c r="A49" s="41"/>
       <c r="B49" s="41"/>
       <c r="C49" s="41"/>
@@ -5721,7 +7740,7 @@
       <c r="H49" s="41"/>
       <c r="I49" s="41"/>
     </row>
-    <row r="50" spans="1:9" ht="39">
+    <row r="50" spans="1:9" ht="39" x14ac:dyDescent="0.45">
       <c r="A50" s="41"/>
       <c r="B50" s="41"/>
       <c r="C50" s="41"/>
@@ -5732,7 +7751,7 @@
       <c r="H50" s="41"/>
       <c r="I50" s="41"/>
     </row>
-    <row r="51" spans="1:9" ht="39">
+    <row r="51" spans="1:9" ht="39" x14ac:dyDescent="0.45">
       <c r="A51" s="41"/>
       <c r="B51" s="41"/>
       <c r="C51" s="41"/>
@@ -5743,7 +7762,7 @@
       <c r="H51" s="41"/>
       <c r="I51" s="41"/>
     </row>
-    <row r="52" spans="1:9" ht="39">
+    <row r="52" spans="1:9" ht="39" x14ac:dyDescent="0.45">
       <c r="A52" s="41"/>
       <c r="B52" s="41"/>
       <c r="C52" s="41"/>
@@ -5754,7 +7773,7 @@
       <c r="H52" s="41"/>
       <c r="I52" s="41"/>
     </row>
-    <row r="53" spans="1:9" ht="39">
+    <row r="53" spans="1:9" ht="39" x14ac:dyDescent="0.45">
       <c r="A53" s="41"/>
       <c r="B53" s="41"/>
       <c r="C53" s="41"/>
@@ -5765,7 +7784,7 @@
       <c r="H53" s="41"/>
       <c r="I53" s="41"/>
     </row>
-    <row r="54" spans="1:9" ht="39">
+    <row r="54" spans="1:9" ht="39" x14ac:dyDescent="0.45">
       <c r="A54" s="41"/>
       <c r="B54" s="41"/>
       <c r="C54" s="41"/>
@@ -5776,7 +7795,7 @@
       <c r="H54" s="41"/>
       <c r="I54" s="41"/>
     </row>
-    <row r="55" spans="1:9" ht="39">
+    <row r="55" spans="1:9" ht="39" x14ac:dyDescent="0.45">
       <c r="A55" s="41"/>
       <c r="B55" s="41"/>
       <c r="C55" s="41"/>
@@ -5787,7 +7806,7 @@
       <c r="H55" s="41"/>
       <c r="I55" s="41"/>
     </row>
-    <row r="56" spans="1:9" ht="39">
+    <row r="56" spans="1:9" ht="39" x14ac:dyDescent="0.45">
       <c r="A56" s="41"/>
       <c r="B56" s="41"/>
       <c r="C56" s="41"/>
@@ -5798,7 +7817,7 @@
       <c r="H56" s="41"/>
       <c r="I56" s="41"/>
     </row>
-    <row r="57" spans="1:9" ht="39">
+    <row r="57" spans="1:9" ht="39" x14ac:dyDescent="0.45">
       <c r="A57" s="41"/>
       <c r="B57" s="41"/>
       <c r="C57" s="41"/>

</xml_diff>